<commit_message>
Digit Span: A, B과제 랜덤화
</commit_message>
<xml_diff>
--- a/template/메인AB.xlsx
+++ b/template/메인AB.xlsx
@@ -1853,7 +1853,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="132">
   <si>
     <t>ID</t>
   </si>
@@ -2187,10 +2187,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[2, 9]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>2-2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2203,34 +2199,18 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[6, 1, 2]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>4-1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[3, 4, 1, 7]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>4-2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[6, 1, 5, 8]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>5-1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[8, 4, 2, 3, 9]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>5-2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2239,66 +2219,34 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[3, 8, 9, 1, 7, 4]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>6-2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[7, 9 ,6, 4, 8, 3]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>7-1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[5, 1, 7, 4, 2, 3, 8]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>7-2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[9, 8, 5, 2, 1, 6, 3]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>8-1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[1, 8, 4, 5, 9, 7, 6, 3]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>8-2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[2, 9, 7, 6, 3, 1, 5, 4]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>9-1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[5, 3, 8, 4, 1, 2, 4, 6, 9]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>9-2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[4, 2, 6, 9, 1, 7, 8, 3, 5]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Reaction Time 1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2336,18 +2284,6 @@
   </si>
   <si>
     <t>stimulus</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[3, 8, 1]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[5, 2, 1, 8, 1]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[4, 1]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2777,7 +2713,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2794,10 +2730,10 @@
         <v>97</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>98</v>
@@ -2844,174 +2780,142 @@
       <c r="A5" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>107</v>
-      </c>
+      <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>147</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>145</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>111</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>113</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>115</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>117</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>146</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>120</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>122</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>124</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>126</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>128</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>130</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>132</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>134</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
@@ -3048,10 +2952,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>1</v>
@@ -3090,10 +2994,10 @@
         <v>26</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>4</v>
@@ -3343,10 +3247,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>96</v>
@@ -3355,10 +3259,10 @@
         <v>42</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>43</v>
@@ -3982,10 +3886,10 @@
         <v>0</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>45</v>
@@ -4064,7 +3968,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>57</v>
@@ -4470,10 +4374,10 @@
         <v>97</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>98</v>
@@ -4527,7 +4431,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -4536,7 +4440,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -4545,7 +4449,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -4554,7 +4458,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -4563,7 +4467,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -4572,7 +4476,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -4581,7 +4485,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -4590,7 +4494,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -4599,7 +4503,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -4608,7 +4512,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -4617,7 +4521,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -4626,7 +4530,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -4635,7 +4539,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -4644,7 +4548,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -4653,7 +4557,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -4692,10 +4596,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>1</v>
@@ -4734,10 +4638,10 @@
         <v>26</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>4</v>
@@ -4956,10 +4860,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>96</v>
@@ -4968,10 +4872,10 @@
         <v>42</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>43</v>
@@ -5002,7 +4906,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>26</v>
@@ -5596,10 +5500,10 @@
         <v>0</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>45</v>
@@ -5678,7 +5582,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>57</v>

</xml_diff>

<commit_message>
Corsi: A, B 과제 랜덤화
</commit_message>
<xml_diff>
--- a/template/메인AB.xlsx
+++ b/template/메인AB.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="12165"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="12165" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Digit Span (A)" sheetId="1" r:id="rId1"/>
@@ -1853,7 +1853,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="116">
   <si>
     <t>ID</t>
   </si>
@@ -1885,24 +1885,15 @@
     <t>4-1</t>
   </si>
   <si>
-    <t>[3, 4, 1, 7]</t>
-  </si>
-  <si>
     <t>4-2</t>
   </si>
   <si>
-    <t>[6, 1, 5, 8]</t>
-  </si>
-  <si>
     <t>5-1</t>
   </si>
   <si>
     <t>5-2</t>
   </si>
   <si>
-    <t>[5, 2, 1, 8, 6]</t>
-  </si>
-  <si>
     <t>6-1</t>
   </si>
   <si>
@@ -1940,45 +1931,6 @@
   </si>
   <si>
     <t>Score</t>
-  </si>
-  <si>
-    <t>[8, 5]</t>
-  </si>
-  <si>
-    <t>[6, 4]</t>
-  </si>
-  <si>
-    <t>[4, 7, 2]</t>
-  </si>
-  <si>
-    <t>[8, 1, 5]</t>
-  </si>
-  <si>
-    <t>[4, 2, 7, 3, 1]</t>
-  </si>
-  <si>
-    <t>[3, 9, 2, 4, 8, 7]</t>
-  </si>
-  <si>
-    <t>[3 ,7 8, 2, 9, 4]</t>
-  </si>
-  <si>
-    <t>[5, 9, 1, 7, 4, 2, 8]</t>
-  </si>
-  <si>
-    <t>[5, 7, 9, 2, 8, 4, 6]</t>
-  </si>
-  <si>
-    <t>[5, 8, 1, 9, 2, 6, 4, 7]</t>
-  </si>
-  <si>
-    <t>[5, 9, 3, 6, 7, 2, 4, 3]</t>
-  </si>
-  <si>
-    <t>[5, 3, 8, 7, 1, 2, 4, 6, 9]</t>
-  </si>
-  <si>
-    <t>[4, 2, 6, 8, 1, 7, 9, 3, 5]</t>
   </si>
   <si>
     <t>반응점수</t>
@@ -2712,7 +2664,7 @@
   </sheetPr>
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
@@ -2727,22 +2679,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -2761,24 +2713,24 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -2787,7 +2739,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -2796,7 +2748,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -2805,7 +2757,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -2814,7 +2766,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -2823,7 +2775,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -2832,7 +2784,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -2841,7 +2793,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -2850,7 +2802,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -2859,7 +2811,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -2868,7 +2820,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -2877,7 +2829,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -2886,7 +2838,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -2895,7 +2847,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -2904,7 +2856,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -2913,7 +2865,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -2933,8 +2885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="B1:C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2952,19 +2904,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G1" s="10"/>
     </row>
@@ -2991,28 +2943,26 @@
         <v>3</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>4</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>29</v>
-      </c>
+      <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
@@ -3023,9 +2973,7 @@
       <c r="A6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>30</v>
-      </c>
+      <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -3036,9 +2984,7 @@
       <c r="A7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>31</v>
-      </c>
+      <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -3049,9 +2995,7 @@
       <c r="A8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>32</v>
-      </c>
+      <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
@@ -3062,9 +3006,7 @@
       <c r="A9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>10</v>
-      </c>
+      <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -3073,11 +3015,9 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>12</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
@@ -3086,11 +3026,9 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>15</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
@@ -3099,11 +3037,9 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>33</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -3112,11 +3048,9 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>34</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
@@ -3125,11 +3059,9 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>35</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
@@ -3138,11 +3070,9 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>36</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
@@ -3151,11 +3081,9 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>37</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
@@ -3164,11 +3092,9 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>38</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
@@ -3177,11 +3103,9 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>39</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
@@ -3190,11 +3114,9 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>40</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
@@ -3203,11 +3125,9 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>41</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
@@ -3247,28 +3167,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -3296,13 +3216,13 @@
         <v>3</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -3886,46 +3806,46 @@
         <v>0</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.3">
@@ -3968,22 +3888,22 @@
         <v>2</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="O4" s="9"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -3993,7 +3913,7 @@
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -4003,7 +3923,7 @@
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -4013,7 +3933,7 @@
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -4023,7 +3943,7 @@
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
@@ -4033,7 +3953,7 @@
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B10" s="6" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
@@ -4043,7 +3963,7 @@
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
@@ -4053,7 +3973,7 @@
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
@@ -4063,7 +3983,7 @@
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B13" s="6" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
@@ -4073,7 +3993,7 @@
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B14" s="6" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -4083,7 +4003,7 @@
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B15" s="6" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
@@ -4093,7 +4013,7 @@
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B16" s="6" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -4103,7 +4023,7 @@
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B17" s="6" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -4113,7 +4033,7 @@
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B18" s="6" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
@@ -4123,7 +4043,7 @@
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B19" s="6" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
@@ -4133,7 +4053,7 @@
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B20" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
@@ -4143,7 +4063,7 @@
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B21" s="6" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
@@ -4153,7 +4073,7 @@
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B22" s="6" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
@@ -4163,7 +4083,7 @@
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B23" s="6" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
@@ -4173,7 +4093,7 @@
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B24" s="6" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -4183,7 +4103,7 @@
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B25" s="6" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
@@ -4193,7 +4113,7 @@
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B26" s="6" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
@@ -4203,7 +4123,7 @@
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B27" s="6" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
@@ -4213,7 +4133,7 @@
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B28" s="6" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
@@ -4223,7 +4143,7 @@
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B29" s="6" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
@@ -4233,7 +4153,7 @@
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B30" s="6" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
@@ -4243,7 +4163,7 @@
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B31" s="6" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
@@ -4253,7 +4173,7 @@
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B32" s="6" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
@@ -4263,7 +4183,7 @@
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B33" s="6" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
@@ -4273,7 +4193,7 @@
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B34" s="6" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
@@ -4283,7 +4203,7 @@
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B35" s="6" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
@@ -4293,7 +4213,7 @@
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B36" s="6" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
@@ -4303,7 +4223,7 @@
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B37" s="6" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
@@ -4313,7 +4233,7 @@
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B38" s="6" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
@@ -4323,7 +4243,7 @@
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B39" s="6" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
@@ -4333,7 +4253,7 @@
     </row>
     <row r="40" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B40" s="6" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
@@ -4371,22 +4291,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -4405,24 +4325,24 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -4431,7 +4351,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -4440,7 +4360,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -4449,7 +4369,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -4458,7 +4378,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -4467,7 +4387,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -4476,7 +4396,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -4485,7 +4405,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -4494,7 +4414,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -4503,7 +4423,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -4512,7 +4432,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -4521,7 +4441,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -4530,7 +4450,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -4539,7 +4459,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -4548,7 +4468,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -4557,7 +4477,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -4596,19 +4516,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G1" s="10"/>
     </row>
@@ -4635,19 +4555,19 @@
         <v>3</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>4</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -4707,7 +4627,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -4718,7 +4638,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -4729,7 +4649,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -4740,7 +4660,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -4751,7 +4671,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -4762,7 +4682,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -4773,7 +4693,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -4784,7 +4704,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -4795,7 +4715,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -4806,7 +4726,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -4817,7 +4737,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -4860,28 +4780,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -4906,16 +4826,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -5500,46 +5420,46 @@
         <v>0</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.3">
@@ -5582,22 +5502,22 @@
         <v>2</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="O4" s="9"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -5607,7 +5527,7 @@
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -5617,7 +5537,7 @@
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -5627,7 +5547,7 @@
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -5637,7 +5557,7 @@
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
@@ -5647,7 +5567,7 @@
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B10" s="6" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
@@ -5657,7 +5577,7 @@
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
@@ -5667,7 +5587,7 @@
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
@@ -5677,7 +5597,7 @@
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B13" s="6" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
@@ -5687,7 +5607,7 @@
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B14" s="6" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -5697,7 +5617,7 @@
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B15" s="6" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
@@ -5707,7 +5627,7 @@
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B16" s="6" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -5717,7 +5637,7 @@
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B17" s="6" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -5727,7 +5647,7 @@
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B18" s="6" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
@@ -5737,7 +5657,7 @@
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B19" s="6" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
@@ -5747,7 +5667,7 @@
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B20" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
@@ -5757,7 +5677,7 @@
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B21" s="6" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
@@ -5767,7 +5687,7 @@
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B22" s="6" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
@@ -5777,7 +5697,7 @@
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B23" s="6" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
@@ -5787,7 +5707,7 @@
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B24" s="6" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -5797,7 +5717,7 @@
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B25" s="6" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
@@ -5807,7 +5727,7 @@
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B26" s="6" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
@@ -5817,7 +5737,7 @@
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B27" s="6" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
@@ -5827,7 +5747,7 @@
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B28" s="6" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
@@ -5837,7 +5757,7 @@
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B29" s="6" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
@@ -5847,7 +5767,7 @@
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B30" s="6" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
@@ -5857,7 +5777,7 @@
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B31" s="6" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
@@ -5867,7 +5787,7 @@
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B32" s="6" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
@@ -5877,7 +5797,7 @@
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B33" s="6" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
@@ -5887,7 +5807,7 @@
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B34" s="6" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
@@ -5897,7 +5817,7 @@
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B35" s="6" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
@@ -5907,7 +5827,7 @@
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B36" s="6" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
@@ -5917,7 +5837,7 @@
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B37" s="6" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
@@ -5927,7 +5847,7 @@
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B38" s="6" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
@@ -5937,7 +5857,7 @@
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B39" s="6" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
@@ -5947,7 +5867,7 @@
     </row>
     <row r="40" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B40" s="6" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>

</xml_diff>